<commit_message>
Updated cnxmod tags to context-cnxmod tags in the quadbase importer and the spreadsheet tagger spec
</commit_message>
<xml_diff>
--- a/spec/fixtures/sample_tags.xlsx
+++ b/spec/fixtures/sample_tags.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
@@ -33,28 +33,28 @@
     <t>Extra Tags</t>
   </si>
   <si>
-    <t>cnxmod:39256206-03b0-4396-abb6-75e6ee5e3c7b</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>filter-type:multi-cnxmod</t>
-  </si>
-  <si>
     <t>lo:stax-phys:1-1-1</t>
   </si>
   <si>
-    <t>cnxmod:102e9604-daa7-4a09-9f9e-232251d1a4ee</t>
-  </si>
-  <si>
-    <t>alternate-cnxmod:39256206-03b0-4396-abb6-75e6ee5e3c7b,cnxmod:102e9604-daa7-4a09-9f9e-232251d1a4ee</t>
-  </si>
-  <si>
     <t>lo:stax-phys:1-2-1,alternate-lo:stax-phys:1-1-1</t>
   </si>
   <si>
     <t>lo:stax-phys:1-2-1,lo:stax-phys:1-2-2</t>
+  </si>
+  <si>
+    <t>context-cnxmod:39256206-03b0-4396-abb6-75e6ee5e3c7b</t>
+  </si>
+  <si>
+    <t>context-cnxmod:102e9604-daa7-4a09-9f9e-232251d1a4ee</t>
+  </si>
+  <si>
+    <t>alternate-context-cnxmod:39256206-03b0-4396-abb6-75e6ee5e3c7b,context-cnxmod:102e9604-daa7-4a09-9f9e-232251d1a4ee</t>
+  </si>
+  <si>
+    <t>filter-type:multi-lo</t>
+  </si>
+  <si>
+    <t>filter-type:multi-cnxmod,filter-type:multi-lo</t>
   </si>
 </sst>
 </file>
@@ -105,8 +105,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -132,7 +134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -143,6 +145,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -153,6 +156,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -485,15 +489,15 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -516,10 +520,10 @@
         <v>-1,-2,-3</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -531,10 +535,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -546,10 +550,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>